<commit_message>
Reestruturação de src, com redução de diretório vertical e adição do diretório analysis
</commit_message>
<xml_diff>
--- a/data/interin/extrato_conta_aplicação_bruto.xlsx
+++ b/data/interin/extrato_conta_aplicação_bruto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,36 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>25/07</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.077.343,87</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>25/08</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>956.265,43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>